<commit_message>
taille de la carte passe a 5 et statiquement
</commit_message>
<xml_diff>
--- a/assets/for_tests/map.xlsx
+++ b/assets/for_tests/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5D1AB9-1F2A-47CD-A731-6861631594FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C99AC-9F95-4CF8-9D2D-4A262317C18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>UN</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>NON</t>
+  </si>
+  <si>
+    <t>assets/for_tests/pikachu.jpeg</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,11 +402,12 @@
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -411,8 +415,14 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -422,8 +432,14 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -432,6 +448,54 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -508,7 +572,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>carte!A1</f>
-        <v>assets/for_tests/img_2.png</v>
+        <v>assets/for_tests/pikachu.jpeg</v>
       </c>
     </row>
   </sheetData>

</xml_diff>